<commit_message>
Correcion de errores y validaciones presentadas en carga de archivo curso
</commit_message>
<xml_diff>
--- a/uploads/educativa/Plantilla_cargarcursoeducativa.xlsx
+++ b/uploads/educativa/Plantilla_cargarcursoeducativa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -1539,8 +1539,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1616,12 +1617,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1644,26 +1653,26 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="B:C"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1686,8 +1695,8 @@
   </sheetPr>
   <dimension ref="A1:A480"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B:C A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1697,7 +1706,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>